<commit_message>
Edited rscripts and excel files
</commit_message>
<xml_diff>
--- a/data/sars_cov2_par.xlsx
+++ b/data/sars_cov2_par.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stellenbosch-my.sharepoint.com/personal/tumelos_sun_ac_za/Documents/Documents/SACEMAProject/Project/Project_Msc/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="230" documentId="11_A636783F555EB5137644B599124867C477AA8E46" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C131AE8F-F6EC-4745-9F93-9EBABE834828}"/>
+  <xr:revisionPtr revIDLastSave="231" documentId="11_A636783F555EB5137644B599124867C477AA8E46" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86E1B931-C21A-432E-AD3C-0D0E3FD78849}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -371,7 +371,7 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>5127592</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="724567" cy="289560"/>
@@ -725,7 +725,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -911,15 +911,19 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>40</v>
+      </c>
+      <c r="D7">
+        <v>12.5</v>
       </c>
       <c r="E7" s="2">
+        <f>1/D7</f>
         <v>0.08</v>
       </c>
       <c r="F7" s="2"/>
@@ -935,20 +939,20 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D8">
-        <v>12.5</v>
+        <v>9</v>
       </c>
       <c r="E8" s="2">
         <f>1/D8</f>
-        <v>0.08</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" t="s">
@@ -958,53 +962,49 @@
         <v>13</v>
       </c>
       <c r="I8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9">
-        <v>9</v>
-      </c>
-      <c r="E9" s="2">
-        <f>1/D9</f>
-        <v>0.1111111111111111</v>
-      </c>
-      <c r="F9" s="2"/>
+        <v>42</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>76</v>
+      </c>
       <c r="G9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H9" t="s">
-        <v>13</v>
+        <v>56</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="I9" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E10" s="5">
-        <v>0.75</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>76</v>
-      </c>
+        <v>0.95</v>
+      </c>
+      <c r="F10" s="5"/>
       <c r="G10" t="s">
         <v>56</v>
       </c>
@@ -1012,21 +1012,24 @@
         <v>6</v>
       </c>
       <c r="I10" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
       </c>
       <c r="E11" s="5">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" t="s">
@@ -1035,25 +1038,22 @@
       <c r="H11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I11" t="s">
-        <v>67</v>
+      <c r="I11" s="2" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" t="s">
-        <v>13</v>
+        <v>75</v>
       </c>
       <c r="E12" s="5">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" t="s">
@@ -1062,68 +1062,68 @@
       <c r="H12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I12" s="2" t="s">
-        <v>79</v>
+      <c r="I12" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="E13" s="5">
-        <v>0.4</v>
+        <v>7</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="6">
+        <v>150000</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" t="s">
         <v>56</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I13" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" t="s">
-        <v>45</v>
-      </c>
-      <c r="E14" s="5">
-        <v>7</v>
-      </c>
-      <c r="F14" s="5"/>
-      <c r="G14" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>33</v>
+      <c r="A15" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" s="6">
-        <v>150000</v>
-      </c>
-      <c r="F15" s="6"/>
+        <v>55</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="F15" s="2"/>
       <c r="G15" t="s">
-        <v>56</v>
+        <v>34</v>
+      </c>
+      <c r="H15" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
saved new figs and modified the scripts
</commit_message>
<xml_diff>
--- a/data/sars_cov2_par.xlsx
+++ b/data/sars_cov2_par.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stellenbosch-my.sharepoint.com/personal/tumelos_sun_ac_za/Documents/Documents/SACEMAProject/Project/Project_Msc/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stellenbosch-my.sharepoint.com/personal/tumelos_sun_ac_za/Documents/Documents/SACEMAProject/My_First_repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="231" documentId="11_A636783F555EB5137644B599124867C477AA8E46" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86E1B931-C21A-432E-AD3C-0D0E3FD78849}"/>
+  <xr:revisionPtr revIDLastSave="238" documentId="11_A636783F555EB5137644B599124867C477AA8E46" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36AC1CED-EF69-477F-8F20-D632283366C6}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -337,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -348,6 +348,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -731,7 +732,7 @@
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="57.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.3984375" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.796875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.69921875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="46.796875" bestFit="1" customWidth="1"/>
@@ -751,7 +752,7 @@
       <c r="D1" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="10" t="s">
         <v>80</v>
       </c>
       <c r="F1" s="7" t="s">
@@ -804,11 +805,11 @@
         <v>36</v>
       </c>
       <c r="D3" s="2">
-        <v>7</v>
-      </c>
-      <c r="E3" s="2">
+        <v>6</v>
+      </c>
+      <c r="E3" s="5">
         <f>1/D3</f>
-        <v>0.14285714285714285</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>73</v>
@@ -834,11 +835,11 @@
         <v>37</v>
       </c>
       <c r="D4">
-        <v>8</v>
-      </c>
-      <c r="E4" s="2">
+        <v>7</v>
+      </c>
+      <c r="E4" s="5">
         <f>1/D4</f>
-        <v>0.125</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>63</v>
@@ -866,7 +867,7 @@
       <c r="D5">
         <v>5</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="5">
         <f>1/D5</f>
         <v>0.2</v>
       </c>
@@ -894,7 +895,7 @@
       <c r="D6">
         <v>3</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="5">
         <f>1/D6</f>
         <v>0.33333333333333331</v>
       </c>
@@ -920,11 +921,11 @@
         <v>40</v>
       </c>
       <c r="D7">
-        <v>12.5</v>
-      </c>
-      <c r="E7" s="2">
+        <v>12</v>
+      </c>
+      <c r="E7" s="5">
         <f>1/D7</f>
-        <v>0.08</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" t="s">
@@ -948,11 +949,11 @@
         <v>41</v>
       </c>
       <c r="D8">
-        <v>9</v>
-      </c>
-      <c r="E8" s="2">
+        <v>18</v>
+      </c>
+      <c r="E8" s="5">
         <f>1/D8</f>
-        <v>0.1111111111111111</v>
+        <v>5.5555555555555552E-2</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" t="s">
@@ -1077,7 +1078,7 @@
         <v>45</v>
       </c>
       <c r="E13" s="5">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" t="s">
@@ -1094,7 +1095,7 @@
       <c r="C14" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="5">
         <v>150000</v>
       </c>
       <c r="F14" s="6"/>
@@ -1112,7 +1113,7 @@
       <c r="C15" t="s">
         <v>55</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="5">
         <v>0.08</v>
       </c>
       <c r="F15" s="2"/>
@@ -1166,7 +1167,6 @@
       <c r="C19" t="s">
         <v>59</v>
       </c>
-      <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="H19" s="2"/>
     </row>

</xml_diff>

<commit_message>
Extended the ps list and adjusted the plots
</commit_message>
<xml_diff>
--- a/data/sars_cov2_par.xlsx
+++ b/data/sars_cov2_par.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stellenbosch-my.sharepoint.com/personal/tumelos_sun_ac_za/Documents/Documents/SACEMAProject/My_First_repo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stellenbosch-my.sharepoint.com/personal/tumelos_sun_ac_za/Documents/Documents/SACEMAProject/Project/Project_Msc/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="238" documentId="11_A636783F555EB5137644B599124867C477AA8E46" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36AC1CED-EF69-477F-8F20-D632283366C6}"/>
@@ -725,8 +725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5279FF3-2450-48F7-BC06-E41D7A5DDB99}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -808,7 +808,7 @@
         <v>6</v>
       </c>
       <c r="E3" s="5">
-        <f>1/D3</f>
+        <f t="shared" ref="E3:E8" si="0">1/D3</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="F3" s="9" t="s">
@@ -838,7 +838,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="5">
-        <f>1/D4</f>
+        <f t="shared" si="0"/>
         <v>0.14285714285714285</v>
       </c>
       <c r="F4" s="2" t="s">
@@ -868,7 +868,7 @@
         <v>5</v>
       </c>
       <c r="E5" s="5">
-        <f>1/D5</f>
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
       <c r="F5" s="2"/>
@@ -896,7 +896,7 @@
         <v>3</v>
       </c>
       <c r="E6" s="5">
-        <f>1/D6</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="F6" s="2"/>
@@ -924,7 +924,7 @@
         <v>12</v>
       </c>
       <c r="E7" s="5">
-        <f>1/D7</f>
+        <f t="shared" si="0"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F7" s="2"/>
@@ -952,7 +952,7 @@
         <v>18</v>
       </c>
       <c r="E8" s="5">
-        <f>1/D8</f>
+        <f t="shared" si="0"/>
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="F8" s="2"/>

</xml_diff>